<commit_message>
Correction of error related to links in Excel
</commit_message>
<xml_diff>
--- a/Project_Management/Sprint2/Burndown chart.xlsx
+++ b/Project_Management/Sprint2/Burndown chart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catarinapedroso/Documents/FCT/2324/ES/sprints/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catarinapedroso/Desktop/projES1/Project_Management/Sprint2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59ACA5A4-5BB3-784F-ADAF-DE0521EEF63F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CFA197-CDDC-6E4B-8C8D-2B67FA42C29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{D17F6CA0-C65A-7D49-8398-913A6E0537C5}"/>
   </bookViews>
@@ -721,7 +721,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'[1]Burndown Chart'!$B$12:$C$12</c:f>
+              <c:f>Sheet1!$B$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -832,7 +832,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'[1]Burndown Chart'!$B$13:$C$13</c:f>
+              <c:f>Sheet1!$B$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -867,7 +867,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'[1]Burndown Chart'!$D$5:$K$5</c:f>
+              <c:f>Sheet1!$D$5:$K$5</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -942,7 +942,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'[1]Burndown Chart'!$B$14:$C$14</c:f>
+              <c:f>Sheet1!$B$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -965,7 +965,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'[1]Burndown Chart'!$D$5:$K$5</c:f>
+              <c:f>Sheet1!$D$5:$K$5</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -2251,8 +2251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4D77F00-F3DE-0743-A902-74A7E0154780}">
   <dimension ref="B1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="110" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M41" sqref="M41"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="110" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2703,31 +2703,31 @@
         <v>0</v>
       </c>
       <c r="E22" s="19">
-        <f>SUM(E6:E21)</f>
+        <f t="shared" ref="E22:K22" si="0">SUM(E6:E21)</f>
         <v>3.85</v>
       </c>
       <c r="F22" s="19">
-        <f>SUM(F6:F21)</f>
+        <f t="shared" si="0"/>
         <v>1.55</v>
       </c>
       <c r="G22" s="19">
-        <f>SUM(G6:G21)</f>
+        <f t="shared" si="0"/>
         <v>1.7</v>
       </c>
       <c r="H22" s="19">
-        <f>SUM(H6:H21)</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
       <c r="I22" s="19">
-        <f>SUM(I6:I21)</f>
+        <f t="shared" si="0"/>
         <v>2.85</v>
       </c>
       <c r="J22" s="19">
-        <f>SUM(J6:J21)</f>
+        <f t="shared" si="0"/>
         <v>2.3000000000000003</v>
       </c>
       <c r="K22" s="19">
-        <f>SUM(K6:K21)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L22" s="20"/>
@@ -2742,31 +2742,31 @@
         <v>15.4</v>
       </c>
       <c r="E23" s="22">
-        <f>D23-E22</f>
+        <f t="shared" ref="E23:K23" si="1">D23-E22</f>
         <v>11.55</v>
       </c>
       <c r="F23" s="23">
-        <f>E23-F22</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="G23" s="23">
-        <f>F23-G22</f>
+        <f t="shared" si="1"/>
         <v>8.3000000000000007</v>
       </c>
       <c r="H23" s="23">
-        <f>G23-H22</f>
+        <f t="shared" si="1"/>
         <v>5.8000000000000007</v>
       </c>
       <c r="I23" s="23">
-        <f>H23-I22</f>
+        <f t="shared" si="1"/>
         <v>2.9500000000000006</v>
       </c>
       <c r="J23" s="24">
-        <f>I23-J22</f>
+        <f t="shared" si="1"/>
         <v>0.65000000000000036</v>
       </c>
       <c r="K23" s="24">
-        <f>J23-K22</f>
+        <f t="shared" si="1"/>
         <v>-0.34999999999999964</v>
       </c>
     </row>

</xml_diff>